<commit_message>
Queda Mongoose y gestion de users
</commit_message>
<xml_diff>
--- a/PracticasSTW/src/p5/funciones.xlsx
+++ b/PracticasSTW/src/p5/funciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Resource</t>
   </si>
@@ -44,9 +44,6 @@
     <t>error</t>
   </si>
   <si>
-    <t>lista de memos</t>
-  </si>
-  <si>
     <t>/memo</t>
   </si>
   <si>
@@ -56,13 +53,43 @@
     <t>new memo</t>
   </si>
   <si>
-    <t>memo con id</t>
-  </si>
-  <si>
-    <t>borrar esta memo</t>
-  </si>
-  <si>
-    <t>borrar todas las memos</t>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>new user</t>
+  </si>
+  <si>
+    <t>user list</t>
+  </si>
+  <si>
+    <t>memo list</t>
+  </si>
+  <si>
+    <t>show memo</t>
+  </si>
+  <si>
+    <t>delete all memo</t>
+  </si>
+  <si>
+    <t>delete this memo</t>
+  </si>
+  <si>
+    <t>update memo</t>
+  </si>
+  <si>
+    <t>delete all users</t>
+  </si>
+  <si>
+    <t>/user/:id</t>
+  </si>
+  <si>
+    <t>show user info</t>
+  </si>
+  <si>
+    <t>update user info</t>
+  </si>
+  <si>
+    <t>delete this user</t>
   </si>
 </sst>
 </file>
@@ -104,8 +131,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,15 +435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -397,10 +453,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -411,36 +467,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>